<commit_message>
No notable change, but new commit?
</commit_message>
<xml_diff>
--- a/metadata.xlsx
+++ b/metadata.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/7ecf4928fe261446/Documents/GitHub/WildCaptive_SeqTech/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="163" documentId="13_ncr:1_{2E4C2DE0-6344-4D58-AFF5-2FD60445EDFF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3BC34784-BD06-4F13-8F37-27EEEB547805}"/>
+  <xr:revisionPtr revIDLastSave="165" documentId="13_ncr:1_{2E4C2DE0-6344-4D58-AFF5-2FD60445EDFF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C6E88455-45FD-41F1-8EDB-9F913833B75B}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{02758EDA-B4C7-4EF1-9F87-DB4E872C78DC}"/>
   </bookViews>
@@ -701,7 +701,7 @@
   <dimension ref="A1:K58"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:K1048576"/>
+      <selection activeCell="A28" activeCellId="6" sqref="A48:XFD51 A38:XFD39 A44:XFD45 A36:XFD37 A5:XFD6 A20:XFD21 A28:XFD29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>